<commit_message>
Add statut warning dans log result nav et kw Add step dans resume de result modif cellStyle dans reesult modif gestoion alert
</commit_message>
<xml_diff>
--- a/TNR/MODELE_RESULTATS_TNR.xlsx
+++ b/TNR/MODELE_RESULTATS_TNR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="6504" windowWidth="28848" windowHeight="6540"/>
+    <workbookView xWindow="-12" yWindow="6504" windowWidth="19140" windowHeight="2844"/>
   </bookViews>
   <sheets>
     <sheet name="RESUME" sheetId="8" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Cas de tests</t>
   </si>
@@ -72,13 +72,31 @@
   </si>
   <si>
     <t>Ticket DE</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>Nombre de STEP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -115,16 +133,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,21 +153,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -171,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -198,20 +193,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,108 +409,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E16"/>
+  <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="27.21875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
+    <col min="3" max="4" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="7"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="8"/>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="15.6">
+    <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="13"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="24" customHeight="1">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:6" ht="24" customHeight="1">
+      <c r="A16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
+    </row>
+    <row r="17" spans="1:1" ht="24.6" customHeight="1">
+      <c r="A17" s="16" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -530,39 +524,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1048576"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="3" max="5" width="11.5546875" style="12"/>
-    <col min="6" max="6" width="48.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="6" width="11.77734375" style="7" customWidth="1"/>
+    <col min="7" max="9" width="11.77734375" style="12" customWidth="1"/>
+    <col min="10" max="10" width="48.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout info context dans result
</commit_message>
<xml_diff>
--- a/TNR/MODELE_RESULTATS_TNR.xlsx
+++ b/TNR/MODELE_RESULTATS_TNR.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Cas de tests</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>Nombre de cas de tests</t>
-  </si>
-  <si>
     <t>Failed</t>
   </si>
   <si>
@@ -59,21 +56,9 @@
     <t>Info contexte</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Version OS</t>
-  </si>
-  <si>
-    <t>Navigateur</t>
-  </si>
-  <si>
     <t>Commentaire</t>
   </si>
   <si>
-    <t>Ticket DE</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
@@ -89,14 +74,44 @@
     <t>WARNING</t>
   </si>
   <si>
-    <t>Nombre de STEP</t>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>STEP</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>Ticket</t>
+  </si>
+  <si>
+    <t>Nom de l'OS</t>
+  </si>
+  <si>
+    <t>Version de l'OS</t>
+  </si>
+  <si>
+    <t>Architecture de l'OS</t>
+  </si>
+  <si>
+    <t>Nom du navigateur</t>
+  </si>
+  <si>
+    <t>Version du navigateur</t>
+  </si>
+  <si>
+    <t>Nombre total de STEP</t>
+  </si>
+  <si>
+    <t>Nombre total de cas de tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -105,13 +120,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -133,8 +141,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +176,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -166,41 +195,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="21" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="21" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,18 +445,18 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D24" sqref="D23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="27.21875" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="4" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6" ht="15.6">
+      <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3"/>
@@ -431,89 +464,93 @@
     <row r="3" spans="1:6">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:6" ht="13.8">
+      <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="10" t="s">
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" ht="13.8">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="10" t="s">
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" ht="13.8">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="B6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" ht="13.8">
       <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="8"/>
-      <c r="B13" s="5"/>
+      <c r="B7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.6">
+      <c r="A8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.8">
+      <c r="A9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="18"/>
+    </row>
+    <row r="10" spans="1:6" ht="13.8">
+      <c r="A10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="18"/>
+    </row>
+    <row r="11" spans="1:6" ht="13.8">
+      <c r="A11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" spans="1:6" ht="13.8">
+      <c r="A12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="18"/>
+    </row>
+    <row r="13" spans="1:6" ht="13.8">
+      <c r="A13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="18"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="15.6">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="16" spans="1:6" ht="24" customHeight="1">
-      <c r="A16" s="14" t="s">
-        <v>10</v>
+      <c r="A16" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="24.6" customHeight="1">
-      <c r="A17" s="16" t="s">
-        <v>24</v>
+      <c r="A17" s="17" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -524,54 +561,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="3" max="6" width="11.77734375" style="7" customWidth="1"/>
-    <col min="7" max="9" width="11.77734375" style="12" customWidth="1"/>
-    <col min="10" max="10" width="48.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
+    <col min="4" max="7" width="10.77734375" style="5" customWidth="1"/>
+    <col min="8" max="10" width="11.77734375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="48.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="15.6">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="15" t="s">
+      <c r="D2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add TC AD.SEC + update
</commit_message>
<xml_diff>
--- a/TNR/MODELE_RESULTATS_TNR.xlsx
+++ b/TNR/MODELE_RESULTATS_TNR.xlsx
@@ -509,9 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
@@ -525,9 +523,9 @@
         <v>7</v>
       </c>
       <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Update RESULT et LOG pour integrer les STEPs
RESULT ajout de styles
RESULT groupe les DETAILS
RESULT gestion des types de STEP
RESULT Renommage du fichier resultat
LOG synchronisation du DateTime avec RESULT : logDate
LOG ajout de addStepInResult
</commit_message>
<xml_diff>
--- a/TNR/MODELE_RESULTATS_TNR.xlsx
+++ b/TNR/MODELE_RESULTATS_TNR.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Cas de tests</t>
   </si>
@@ -23,12 +23,6 @@
     <t>Résultat</t>
   </si>
   <si>
-    <t>Heure fin</t>
-  </si>
-  <si>
-    <t>Heure début</t>
-  </si>
-  <si>
     <t>Durée</t>
   </si>
   <si>
@@ -111,13 +105,24 @@
   </si>
   <si>
     <t>Base de donnée</t>
+  </si>
+  <si>
+    <t>Date Time</t>
+  </si>
+  <si>
+    <t>Heure
+début</t>
+  </si>
+  <si>
+    <t>Heure
+fin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -187,6 +192,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -230,16 +242,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -249,12 +257,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -299,6 +301,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,186 +539,186 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="A7" s="10"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="18" customHeight="1">
+      <c r="A8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1">
+      <c r="A9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1">
+      <c r="A10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1">
+      <c r="A11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1">
+      <c r="A12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1">
+      <c r="A13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1">
+      <c r="A14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1">
+      <c r="A15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1">
+      <c r="A16" s="11"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" ht="18" customHeight="1">
+      <c r="A17" s="20"/>
+      <c r="B17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
-      <c r="A5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
-      <c r="A6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="18" customHeight="1">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="19" t="s">
+      <c r="D17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.95" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" ht="24.6" customHeight="1">
+      <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
-      <c r="A13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1">
-      <c r="A14" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="18" customHeight="1">
-      <c r="A17" s="24"/>
-      <c r="B17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="25.95" customHeight="1">
-      <c r="A18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" ht="24.6" customHeight="1">
-      <c r="A19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -708,79 +728,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="90.77734375" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="7" width="10.77734375" style="2" customWidth="1"/>
-    <col min="8" max="10" width="11.77734375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="48.77734375" customWidth="1"/>
+    <col min="4" max="4" width="4.77734375" customWidth="1"/>
+    <col min="5" max="8" width="4.77734375" style="2" customWidth="1"/>
+    <col min="9" max="11" width="8.77734375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="58.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6">
+    <row r="1" spans="1:13" ht="15.6">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="L1" s="1"/>
+      <c r="M1" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="51.6">
+      <c r="A2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="26" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean stable + ecran xml
</commit_message>
<xml_diff>
--- a/TNR/MODELE_RESULTATS_TNR.xlsx
+++ b/TNR/MODELE_RESULTATS_TNR.xlsx
@@ -324,39 +324,39 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="21" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="21" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,9 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:G16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
@@ -582,54 +580,54 @@
       <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="A7" s="6"/>
@@ -653,89 +651,89 @@
       <c r="A9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1">
       <c r="A14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:7" ht="25.95" customHeight="1"/>
     <row r="18" spans="1:7" ht="25.95" customHeight="1">
@@ -755,29 +753,29 @@
       <c r="F18" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="32"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="24.6" customHeight="1">
       <c r="A19" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="32"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="32"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
DevOps et desired capabilities
Ajout de desired capabilities de Chrome headless
Ajout de DEVOPS_TICKET_CREATION dans les properties
modif des liens des screenshot
Ajout du lien de la tache
Modif des info history et comment des Task et Bug
</commit_message>
<xml_diff>
--- a/TNR/MODELE_RESULTATS_TNR.xlsx
+++ b/TNR/MODELE_RESULTATS_TNR.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Cas de tests</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev Ops Task N° </t>
   </si>
 </sst>
 </file>
@@ -268,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -334,9 +337,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -354,20 +354,26 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,7 +582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G20"/>
+  <dimension ref="A2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -587,60 +593,65 @@
     <col min="3" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="25.9" customHeight="1">
+    <row r="2" spans="1:10" ht="25.9" customHeight="1">
       <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
+      <c r="B2" s="26"/>
+      <c r="C2" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
+      <c r="B3" s="27"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
+      <c r="B4" s="28"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1">
       <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1">
+      <c r="B5" s="28"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1">
+      <c r="B6" s="28"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
@@ -648,7 +659,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="18" customHeight="1">
+    <row r="8" spans="1:10" ht="18" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
@@ -658,7 +669,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1">
+    <row r="9" spans="1:10" ht="15" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>18</v>
       </c>
@@ -669,7 +680,7 @@
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1">
+    <row r="10" spans="1:10" ht="15" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
@@ -680,7 +691,7 @@
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1">
+    <row r="11" spans="1:10" ht="15" customHeight="1">
       <c r="A11" s="15" t="s">
         <v>20</v>
       </c>
@@ -691,7 +702,7 @@
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
+    <row r="12" spans="1:10" ht="15" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
@@ -702,7 +713,7 @@
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1">
+    <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>22</v>
       </c>
@@ -713,38 +724,38 @@
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1">
+    <row r="14" spans="1:10" ht="15" customHeight="1">
       <c r="A14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1">
       <c r="A15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" spans="1:7" ht="25.9" customHeight="1"/>
     <row r="18" spans="1:7" ht="25.9" customHeight="1">
@@ -764,35 +775,36 @@
       <c r="F18" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="25"/>
+      <c r="G18" s="24"/>
     </row>
     <row r="19" spans="1:7" ht="24.6" customHeight="1">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:J2"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="B16:G16"/>
-    <mergeCell ref="D2:G2"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B11:G11"/>
@@ -824,8 +836,9 @@
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
     <col min="5" max="8" width="4.7109375" style="2" customWidth="1"/>
     <col min="9" max="11" width="8.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="55.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="70.7109375" style="30" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75">

</xml_diff>